<commit_message>
Add fsm to infrared
</commit_message>
<xml_diff>
--- a/egg-fsm.xlsx
+++ b/egg-fsm.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="19180" windowHeight="3460"/>
+    <workbookView activeTab="0" windowWidth="19180" windowHeight="8860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1" count="1">
-  <si>
-    <t>state\event</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4" count="4">
+  <si>
+    <t>lock on\LOCKING ON</t>
+  </si>
+  <si>
+    <t>play 1m timeout\</t>
+  </si>
+  <si>
+    <t>play 2m timeout\</t>
+  </si>
+  <si>
+    <t>play 3m timeout
+lock on\LOCKING ON</t>
   </si>
 </sst>
 </file>
@@ -88,11 +98,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0" tabSelected="1">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D7" sqref="D7"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -103,89 +113,112 @@
     <col min="5" max="5" style="0" width="15.213371394230771" bestFit="1" customWidth="1"/>
     <col min="6" max="6" style="0" width="16.141887019230772" bestFit="1" customWidth="1"/>
     <col min="7" max="7" style="0" width="17.07040264423077" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" style="0" width="9.142307692307693"/>
+    <col min="8" max="8" style="0" width="12.42782451923077" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>state\event</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>LOCK OFF</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>LOCK ON</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>INFRARED TRIGGERED</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>1 MINUTE TIMEOUT</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>2 MINUTES TIMEOUT</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>3 MINUTES TIMEOUT</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>DELAY TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="19.875">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>LOCKING ON</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>play welcome
+lock off\DELAYING</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="19.875">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DELAYING</t>
+        </is>
+      </c>
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>LOCK OFF</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>LOCK ON</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>INFRARED TRIGGERED</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>1 MINUTE TIMEOUT</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>2 MINUTES TIMEOUT</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>3 MINUTES TIMEOUT</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="19.875">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>LOCKING ON</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>play welcome
-lock off\LOCKING OFF</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="19.875">
-      <c r="A3" t="inlineStr">
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>\LOCKING OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="19.875">
+      <c r="A4" t="inlineStr">
         <is>
           <t>LOCKING OFF</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>lock on\LOCKING ON</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>play goodbye
 lock on\LOCKING ON</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>play 1m timeout\</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>play 2m timeout\</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>play 3m timeout
-lock on\LOCKING ON</t>
-        </is>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report fallen event to epigyny
</commit_message>
<xml_diff>
--- a/egg-fsm.xlsx
+++ b/egg-fsm.xlsx
@@ -25,19 +25,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4" count="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2" count="2">
   <si>
     <t>lock on\LOCKING ON</t>
   </si>
   <si>
-    <t>play 1m timeout\</t>
-  </si>
-  <si>
-    <t>play 2m timeout\</t>
-  </si>
-  <si>
-    <t>play 3m timeout
-lock on\LOCKING ON</t>
+    <t>play goodbye
+lock on
+fallen\LOCKING ON</t>
   </si>
 </sst>
 </file>
@@ -98,22 +93,21 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="10.570793269230771" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" style="0" width="18.92743389423077" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="0" width="13.35634014423077" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" style="0" width="16.141887019230772" bestFit="1" customWidth="1"/>
     <col min="3" max="4" style="0" width="17.07040264423077" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" style="0" width="15.213371394230771" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" style="0" width="16.141887019230772" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" style="0" width="20.784465144230772" bestFit="1" customWidth="1"/>
     <col min="7" max="7" style="0" width="17.07040264423077" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" style="0" width="12.42782451923077" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" style="0" width="14.28485576923077" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
@@ -172,7 +166,7 @@
         </is>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19.875">
+    <row r="3" spans="1:8">
       <c r="A3" t="inlineStr">
         <is>
           <t>DELAYING</t>
@@ -181,44 +175,65 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>\LOCKING OFF</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="19.875">
+          <t>\LOCKING OFF 1M</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="29.625">
       <c r="A4" t="inlineStr">
         <is>
-          <t>LOCKING OFF</t>
+          <t>LOCKING OFF 1M</t>
         </is>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>play goodbye
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>play 1m\LOCKING OFF 2M</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="29.625">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>LOCKING OFF 2M</t>
+        </is>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>play 2m\LOCKING OFF 3M</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="29.625">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>LOCKING OFF 3M</t>
+        </is>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>play 3m
 lock on\LOCKING ON</t>
         </is>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adapte new uart3 packet protocol and reverse lock and infrared ports
</commit_message>
<xml_diff>
--- a/egg-fsm.xlsx
+++ b/egg-fsm.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="19180" windowHeight="8860"/>
+    <workbookView activeTab="0" windowWidth="19180" windowHeight="8440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,15 +27,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3" count="3">
   <si>
+    <t>state\event</t>
+  </si>
+  <si>
     <t>lock on\LOCKING ON</t>
   </si>
   <si>
     <t>play goodbye
 lock on
 fallen\LOCKING ON</t>
-  </si>
-  <si>
-    <t>play 1m\LOCKING OFF 2M</t>
   </si>
 </sst>
 </file>
@@ -99,27 +99,25 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H8" sqref="H8"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="14.28485576923077" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" style="0" width="16.141887019230772" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" style="0" width="17.07040264423077" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" style="0" width="21.71298076923077" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" style="0" width="20.784465144230772" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" style="0" width="17.07040264423077" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" style="0" width="15.213371394230771" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="0" width="15.713341346153848" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" style="0" width="17.713221153846156" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" style="0" width="18.71316105769231" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" style="0" width="23.71286057692308" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" style="0" width="22.712920673076926" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" style="0" width="18.71316105769231" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" style="0" width="16.71328125" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>state\event</t>
-        </is>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
@@ -162,7 +160,7 @@
         </is>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.875">
+    <row r="2" spans="1:9" ht="23.25">
       <c r="A2" t="inlineStr">
         <is>
           <t>LOCKING ON</t>
@@ -175,14 +173,14 @@
         </is>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="12">
       <c r="A3" t="inlineStr">
         <is>
           <t>DELAYING</t>
         </is>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -190,17 +188,17 @@
         </is>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="29.625">
+    <row r="4" spans="1:9" ht="34.5">
       <c r="A4" t="inlineStr">
         <is>
           <t>LOCKING OFF 30S</t>
         </is>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -208,33 +206,35 @@
         </is>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="29.625">
+    <row r="5" spans="1:9" ht="34.5">
       <c r="A5" t="inlineStr">
         <is>
           <t>LOCKING OFF 1M</t>
         </is>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="29.625">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>play 1m\LOCKING OFF 2M</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="34.5">
       <c r="A6" t="inlineStr">
         <is>
           <t>LOCKING OFF 2M</t>
         </is>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -242,17 +242,17 @@
         </is>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="29.625">
+    <row r="7" spans="1:9" ht="34.5">
       <c r="A7" t="inlineStr">
         <is>
           <t>LOCKING OFF 3M</t>
         </is>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Play fallen audio when infrared triggered at locking on state
</commit_message>
<xml_diff>
--- a/egg-fsm.xlsx
+++ b/egg-fsm.xlsx
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3" count="3">
-  <si>
-    <t>state\event</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2" count="2">
   <si>
     <t>lock on\LOCKING ON</t>
   </si>
@@ -100,7 +97,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G7" sqref="G7"/>
+      <selection pane="topRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -116,8 +113,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>state\event</t>
+        </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
@@ -160,7 +159,7 @@
         </is>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="23.25">
+    <row r="2" spans="1:9" ht="34.5">
       <c r="A2" t="inlineStr">
         <is>
           <t>LOCKING ON</t>
@@ -172,6 +171,13 @@
 lock off\DELAYING</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>play fallen
+lock on
+fallen\LOCKING ON</t>
+        </is>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="12">
       <c r="A3" t="inlineStr">
@@ -180,7 +186,7 @@
         </is>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -195,10 +201,10 @@
         </is>
       </c>
       <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -213,10 +219,10 @@
         </is>
       </c>
       <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
         <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -231,10 +237,10 @@
         </is>
       </c>
       <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
         <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -249,10 +255,10 @@
         </is>
       </c>
       <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
         <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>

</xml_diff>